<commit_message>
Update Merge Class and database
</commit_message>
<xml_diff>
--- a/Database/Data_20150722/Teachers.xlsx
+++ b/Database/Data_20150722/Teachers.xlsx
@@ -14,25 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
-  <si>
-    <t>LoanNTP</t>
-  </si>
-  <si>
-    <t>TamNT</t>
-  </si>
-  <si>
-    <t>DungDV</t>
-  </si>
-  <si>
-    <t>NguyenLTT</t>
-  </si>
-  <si>
-    <t>HaiNM</t>
-  </si>
-  <si>
-    <t>DungNT3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
   <si>
     <t>ChiLP</t>
   </si>
@@ -49,42 +31,12 @@
     <t>TrungNT</t>
   </si>
   <si>
-    <t>TrungTT</t>
-  </si>
-  <si>
-    <t>NgaNTT</t>
-  </si>
-  <si>
-    <t>LinhLHM</t>
-  </si>
-  <si>
-    <t>ChinhVV</t>
-  </si>
-  <si>
-    <t>NamVX</t>
-  </si>
-  <si>
-    <t>QuyenTTL</t>
-  </si>
-  <si>
-    <t>NamPT</t>
-  </si>
-  <si>
     <t>HaNS2</t>
   </si>
   <si>
     <t>DucHM2</t>
   </si>
   <si>
-    <t>HoaiNV</t>
-  </si>
-  <si>
-    <t>LucPT</t>
-  </si>
-  <si>
-    <t>LanTV</t>
-  </si>
-  <si>
     <t>SonHX</t>
   </si>
   <si>
@@ -97,42 +49,15 @@
     <t>CuongN</t>
   </si>
   <si>
-    <t>CuongN1</t>
-  </si>
-  <si>
-    <t>CuongN2</t>
-  </si>
-  <si>
     <t>TrungDT</t>
   </si>
   <si>
     <t>MaiVTT</t>
   </si>
   <si>
-    <t>VietTK</t>
-  </si>
-  <si>
-    <t>HaiDT</t>
-  </si>
-  <si>
-    <t>CongLT</t>
-  </si>
-  <si>
-    <t>ThanhVC</t>
-  </si>
-  <si>
-    <t>HieuTM</t>
-  </si>
-  <si>
-    <t>HoangNM</t>
-  </si>
-  <si>
     <t>MaiTT</t>
   </si>
   <si>
-    <t>CuongDM</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -142,54 +67,15 @@
     <t>Email</t>
   </si>
   <si>
-    <t>LoanNTP@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>TamNT@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>DungDV@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>CuongDM@fpt.edu.vn</t>
-  </si>
-  <si>
     <t>MaiTT@fpt.edu.vn</t>
   </si>
   <si>
-    <t>HaiNM@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>HoangNM@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>HieuTM@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>ThanhVC@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>CongLT@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>HaiDT@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>VietTK@fpt.edu.vn</t>
-  </si>
-  <si>
     <t>MaiVTT@fpt.edu.vn</t>
   </si>
   <si>
     <t>TrungDT@fpt.edu.vn</t>
   </si>
   <si>
-    <t>CuongN2@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>CuongN1@fpt.edu.vn</t>
-  </si>
-  <si>
     <t>CuongN@fpt.edu.vn</t>
   </si>
   <si>
@@ -202,12 +88,6 @@
     <t>SonHX@fpt.edu.vn</t>
   </si>
   <si>
-    <t>NguyenLTT@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>DungNT3@fpt.edu.vn</t>
-  </si>
-  <si>
     <t>ChiLP@fpt.edu.vn</t>
   </si>
   <si>
@@ -223,46 +103,130 @@
     <t>TrungNT@fpt.edu.vn</t>
   </si>
   <si>
-    <t>TrungTT@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>LanTV@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>LucPT@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>HoaiNV@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>NamPT@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>QuyenTTL@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>NamVX@fpt.edu.vn</t>
-  </si>
-  <si>
     <t>DucHM2@fpt.edu.vn</t>
   </si>
   <si>
     <t>HaNS2@fpt.edu.vn</t>
   </si>
   <si>
-    <t>ChinhVV@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>LinhLHM@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>NgaNTT@fpt.edu.vn</t>
-  </si>
-  <si>
     <t>Account Type</t>
   </si>
   <si>
     <t>teacher</t>
+  </si>
+  <si>
+    <t>CongLT2</t>
+  </si>
+  <si>
+    <t>HoaiNV2</t>
+  </si>
+  <si>
+    <t>HoaiNV2@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>DungLM</t>
+  </si>
+  <si>
+    <t>HuongNT7</t>
+  </si>
+  <si>
+    <t>TrungNQ</t>
+  </si>
+  <si>
+    <t>KhuongPD</t>
+  </si>
+  <si>
+    <t>SangNV</t>
+  </si>
+  <si>
+    <t>AnhPT</t>
+  </si>
+  <si>
+    <t>HienDTT</t>
+  </si>
+  <si>
+    <t>BangBH</t>
+  </si>
+  <si>
+    <t>LamPT</t>
+  </si>
+  <si>
+    <t>BinhNV2</t>
+  </si>
+  <si>
+    <t>ThuLX</t>
+  </si>
+  <si>
+    <t>VietNK</t>
+  </si>
+  <si>
+    <t>DuanTC</t>
+  </si>
+  <si>
+    <t>VanDT</t>
+  </si>
+  <si>
+    <t>QuyPH</t>
+  </si>
+  <si>
+    <t>DungNT</t>
+  </si>
+  <si>
+    <t>HuyenTT</t>
+  </si>
+  <si>
+    <t>DungLM@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>HuyenTT@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>DungNT@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>QuyPH@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>VanDT@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>DuanTC@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>VietNK@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>ThuLX@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>BinhNV2@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>LamPT@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>BangBH@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>HienDTT@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>CongLT2@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>AnhPT@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>SangNV@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>KhuongPD@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>TrungNQ@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>HuongNT7@fpt.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -615,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,128 +593,128 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,24 +725,24 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -789,10 +753,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -803,446 +767,341 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C41" r:id="rId4"/>
-    <hyperlink ref="C40" r:id="rId5"/>
-    <hyperlink ref="C39" r:id="rId6"/>
-    <hyperlink ref="C38" r:id="rId7"/>
-    <hyperlink ref="C37" r:id="rId8"/>
-    <hyperlink ref="C36" r:id="rId9"/>
-    <hyperlink ref="C35" r:id="rId10"/>
-    <hyperlink ref="C34" r:id="rId11"/>
-    <hyperlink ref="C33" r:id="rId12"/>
-    <hyperlink ref="C32" r:id="rId13"/>
-    <hyperlink ref="C31" r:id="rId14"/>
-    <hyperlink ref="C30" r:id="rId15"/>
-    <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C28" r:id="rId17"/>
-    <hyperlink ref="C27" r:id="rId18"/>
-    <hyperlink ref="C26" r:id="rId19"/>
-    <hyperlink ref="C25" r:id="rId20"/>
-    <hyperlink ref="C5" r:id="rId21"/>
-    <hyperlink ref="C6" r:id="rId22"/>
-    <hyperlink ref="C7" r:id="rId23"/>
-    <hyperlink ref="C8" r:id="rId24"/>
-    <hyperlink ref="C9" r:id="rId25"/>
-    <hyperlink ref="C10" r:id="rId26"/>
+    <hyperlink ref="C33" r:id="rId2"/>
+    <hyperlink ref="C32" r:id="rId3"/>
+    <hyperlink ref="C31" r:id="rId4"/>
+    <hyperlink ref="C30" r:id="rId5"/>
+    <hyperlink ref="C29" r:id="rId6"/>
+    <hyperlink ref="C28" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId8"/>
+    <hyperlink ref="C4" r:id="rId9"/>
+    <hyperlink ref="C34" r:id="rId10"/>
+    <hyperlink ref="C27" r:id="rId11"/>
+    <hyperlink ref="C26" r:id="rId12"/>
+    <hyperlink ref="C25" r:id="rId13"/>
+    <hyperlink ref="C24" r:id="rId14"/>
+    <hyperlink ref="C23" r:id="rId15"/>
+    <hyperlink ref="C22" r:id="rId16"/>
+    <hyperlink ref="C21" r:id="rId17"/>
+    <hyperlink ref="C20" r:id="rId18"/>
+    <hyperlink ref="C19" r:id="rId19"/>
+    <hyperlink ref="C18" r:id="rId20"/>
+    <hyperlink ref="C17" r:id="rId21"/>
+    <hyperlink ref="C16" r:id="rId22"/>
+    <hyperlink ref="C15" r:id="rId23"/>
+    <hyperlink ref="C14" r:id="rId24"/>
+    <hyperlink ref="C13" r:id="rId25"/>
+    <hyperlink ref="C12" r:id="rId26"/>
     <hyperlink ref="C11" r:id="rId27"/>
-    <hyperlink ref="C12" r:id="rId28"/>
-    <hyperlink ref="C13" r:id="rId29"/>
-    <hyperlink ref="C24" r:id="rId30"/>
-    <hyperlink ref="C23" r:id="rId31"/>
-    <hyperlink ref="C22" r:id="rId32"/>
-    <hyperlink ref="C21" r:id="rId33"/>
-    <hyperlink ref="C20" r:id="rId34"/>
-    <hyperlink ref="C19" r:id="rId35"/>
-    <hyperlink ref="C18" r:id="rId36"/>
-    <hyperlink ref="C17" r:id="rId37"/>
-    <hyperlink ref="C16" r:id="rId38"/>
-    <hyperlink ref="C15" r:id="rId39"/>
-    <hyperlink ref="C14" r:id="rId40"/>
+    <hyperlink ref="C5" r:id="rId28"/>
+    <hyperlink ref="C6" r:id="rId29"/>
+    <hyperlink ref="C7" r:id="rId30"/>
+    <hyperlink ref="C8" r:id="rId31"/>
+    <hyperlink ref="C9" r:id="rId32"/>
+    <hyperlink ref="C10" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>